<commit_message>
Exception Handling in Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Test Automation\SeleniumAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABB04B9-31F0-4024-8C8D-A16ED83F66D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC37D3FA-1045-4BFE-B25A-B5004477F88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>testname</t>
   </si>
@@ -122,6 +122,21 @@
   </si>
   <si>
     <t>billingAddress</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>menuText</t>
+  </si>
+  <si>
+    <t>Store</t>
   </si>
 </sst>
 </file>
@@ -493,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -514,25 +529,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFDBB96-E624-47AD-9346-29C8C1FA2E48}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,37 +555,43 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -578,14 +599,14 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
@@ -607,8 +628,14 @@
       <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -616,14 +643,14 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="2" t="s">
         <v>26</v>
       </c>
@@ -645,8 +672,14 @@
       <c r="L3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -654,42 +687,93 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{CD286DEF-AEB3-4FB9-BEEE-35313ED4DB10}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{09C20DE4-E0E1-46AC-BC9C-B5195EF05E6C}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{766C230E-87DA-4504-85B7-D9044A8A1506}"/>
-    <hyperlink ref="J4" r:id="rId4" xr:uid="{569DE1A8-D31E-454B-80E9-8B878F8496F9}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{CD286DEF-AEB3-4FB9-BEEE-35313ED4DB10}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{09C20DE4-E0E1-46AC-BC9C-B5195EF05E6C}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{766C230E-87DA-4504-85B7-D9044A8A1506}"/>
+    <hyperlink ref="K4" r:id="rId4" xr:uid="{569DE1A8-D31E-454B-80E9-8B878F8496F9}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{0EB51EE4-857D-4ADC-85E5-75E4CF54DCE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added Decoder functionality to decode password
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Test Automation\SeleniumAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC37D3FA-1045-4BFE-B25A-B5004477F88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAB7050-99E3-4D9D-9E04-A7B911AA8EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>singhabhi04</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Store</t>
+  </si>
+  <si>
+    <t>VGVzdEAxMjM=</t>
   </si>
 </sst>
 </file>
@@ -181,10 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -531,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFDBB96-E624-47AD-9346-29C8C1FA2E48}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -564,31 +565,31 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -599,40 +600,40 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -643,40 +644,40 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -687,40 +688,40 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -731,49 +732,46 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{CD286DEF-AEB3-4FB9-BEEE-35313ED4DB10}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{09C20DE4-E0E1-46AC-BC9C-B5195EF05E6C}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{766C230E-87DA-4504-85B7-D9044A8A1506}"/>
-    <hyperlink ref="K4" r:id="rId4" xr:uid="{569DE1A8-D31E-454B-80E9-8B878F8496F9}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{0EB51EE4-857D-4ADC-85E5-75E4CF54DCE6}"/>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{569DE1A8-D31E-454B-80E9-8B878F8496F9}"/>
+    <hyperlink ref="E2:E5" r:id="rId2" display="test@ram.com" xr:uid="{0AEB3F4D-5E1A-4782-8DB1-A3D57AFD0569}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>